<commit_message>
trying to create a new cleaner script for graphs and plots
</commit_message>
<xml_diff>
--- a/Pena_2025.xlsx
+++ b/Pena_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthapena/Desktop/Project/Brooks_lake_2025/Cyanotoxins_2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthapena/Desktop/Project/Brooks_lake_2025/CODE/cyanotoxin/Cyanotoxins_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB9AF74-2B65-8E42-AD64-E56D6EE01CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B3C6F1-365E-164F-BABD-6F7B830C8217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13224,8 +13224,8 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
-      <selection activeCell="J404" sqref="J404"/>
+    <sheetView tabSelected="1" topLeftCell="A410" workbookViewId="0">
+      <selection activeCell="C379" sqref="C379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -21498,7 +21498,7 @@
         <v>38</v>
       </c>
       <c r="C401" s="42">
-        <v>42276</v>
+        <v>45929</v>
       </c>
       <c r="D401" s="40" t="s">
         <v>50</v>

</xml_diff>